<commit_message>
Set up adjacency tests, added some tests on the xlsx
</commit_message>
<xml_diff>
--- a/MapOfCampusCLUE TESTS.xlsx
+++ b/MapOfCampusCLUE TESTS.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\datwh\Documents\College\Sophmore\Spring\Soft E\Labs\Clue\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabeh\Documents\USB backup\Spring 2021\Software Engineering\eclipse-workspace\Clue\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0D54CB4-42E5-48EC-BA97-F384B45A8EC1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89601B3F-5DB4-4928-990D-D7511564D75F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{FEEFAB7E-8D71-41ED-9D3E-D1228D75F521}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{FEEFAB7E-8D71-41ED-9D3E-D1228D75F521}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -647,34 +647,34 @@
   <dimension ref="A1:AD27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AD12" sqref="AD12"/>
+      <selection activeCell="AC21" sqref="AC21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="3.26953125" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="3.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="3.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="3.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="2.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="3.81640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="3.08984375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="3.36328125" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="3.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.265625" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="3.796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="3.265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="3.796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="2.796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="3.796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="3.06640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="3.265625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="3.81640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="3.26953125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="3.81640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="3.26953125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="3.36328125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="3.26953125" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="3.81640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="3.36328125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="3.26953125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="43.54296875" customWidth="1"/>
+    <col min="16" max="17" width="3.796875" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="3.265625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="3.796875" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="3.265625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="3.265625" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="3.796875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="3.265625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="43.53125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:30" s="12" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B1" s="12">
         <v>0</v>
       </c>
@@ -760,7 +760,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A2" s="12">
         <v>0</v>
       </c>
@@ -849,7 +849,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A3" s="12">
         <v>1</v>
       </c>
@@ -938,7 +938,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A4" s="12">
         <v>2</v>
       </c>
@@ -1024,7 +1024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A5" s="12">
         <v>3</v>
       </c>
@@ -1113,7 +1113,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A6" s="12">
         <v>4</v>
       </c>
@@ -1202,7 +1202,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A7" s="12">
         <v>5</v>
       </c>
@@ -1288,7 +1288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A8" s="12">
         <v>6</v>
       </c>
@@ -1377,7 +1377,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A9" s="12">
         <v>7</v>
       </c>
@@ -1466,7 +1466,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A10" s="12">
         <v>8</v>
       </c>
@@ -1552,7 +1552,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A11" s="12">
         <v>9</v>
       </c>
@@ -1638,7 +1638,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A12" s="12">
         <v>10</v>
       </c>
@@ -1724,7 +1724,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A13" s="12">
         <v>11</v>
       </c>
@@ -1810,7 +1810,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A14" s="12">
         <v>12</v>
       </c>
@@ -1859,7 +1859,7 @@
       <c r="P14" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="Q14" s="7" t="s">
+      <c r="Q14" s="19" t="s">
         <v>6</v>
       </c>
       <c r="R14" s="7" t="s">
@@ -1896,7 +1896,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A15" s="12">
         <v>13</v>
       </c>
@@ -1982,7 +1982,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A16" s="12">
         <v>14</v>
       </c>
@@ -2068,7 +2068,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A17" s="12">
         <v>15</v>
       </c>
@@ -2154,7 +2154,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A18" s="12">
         <v>16</v>
       </c>
@@ -2240,7 +2240,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A19" s="12">
         <v>17</v>
       </c>
@@ -2326,7 +2326,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A20" s="12">
         <v>18</v>
       </c>
@@ -2412,7 +2412,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A21" s="12">
         <v>19</v>
       </c>
@@ -2498,7 +2498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A22" s="12">
         <v>20</v>
       </c>
@@ -2584,7 +2584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A23" s="12">
         <v>21</v>
       </c>
@@ -2670,7 +2670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A24" s="12">
         <v>22</v>
       </c>
@@ -2756,7 +2756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A25" s="12">
         <v>23</v>
       </c>
@@ -2842,7 +2842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A26" s="12">
         <v>24</v>
       </c>
@@ -2928,7 +2928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A27" s="12">
         <v>25</v>
       </c>

</xml_diff>

<commit_message>
Added target tests and fixed junit errors in adjacey, added to board and boardcell to fix errors
</commit_message>
<xml_diff>
--- a/MapOfCampusCLUE TESTS.xlsx
+++ b/MapOfCampusCLUE TESTS.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabeh\Documents\USB backup\Spring 2021\Software Engineering\eclipse-workspace\Clue\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\datwh\Documents\College\Sophmore\Spring\Soft E\Labs\Clue\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89601B3F-5DB4-4928-990D-D7511564D75F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{143269BE-7C9A-4EF3-8751-C211D92B2A1B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{FEEFAB7E-8D71-41ED-9D3E-D1228D75F521}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{FEEFAB7E-8D71-41ED-9D3E-D1228D75F521}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -299,7 +299,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -322,7 +322,6 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -647,34 +646,34 @@
   <dimension ref="A1:AD27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AC21" sqref="AC21"/>
+      <selection activeCell="AC11" sqref="AC11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.265625" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="3.796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="3.265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="3.796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="2.796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="3.796875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="3.06640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="3.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="3.265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.26953125" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="3.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="3.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="3.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="2.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="3.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="3.08984375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="3.36328125" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="3.26953125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="3.796875" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="3.265625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="3.796875" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="3.265625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="3.33203125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="3.265625" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="3.796875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="3.33203125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="3.265625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="43.53125" customWidth="1"/>
+    <col min="16" max="17" width="3.81640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="3.26953125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="3.81640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="3.26953125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="3.36328125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="3.26953125" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="3.81640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="3.36328125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="3.26953125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="43.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="12" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:30" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B1" s="12">
         <v>0</v>
       </c>
@@ -760,7 +759,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A2" s="12">
         <v>0</v>
       </c>
@@ -770,7 +769,7 @@
       <c r="C2" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="D2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E2" s="2" t="s">
@@ -849,7 +848,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A3" s="12">
         <v>1</v>
       </c>
@@ -938,17 +937,17 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A4" s="12">
         <v>2</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="21" t="s">
         <v>3</v>
       </c>
       <c r="E4" s="8" t="s">
@@ -1024,7 +1023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A5" s="12">
         <v>3</v>
       </c>
@@ -1076,7 +1075,7 @@
       <c r="Q5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="R5" s="20" t="s">
+      <c r="R5" s="7" t="s">
         <v>6</v>
       </c>
       <c r="S5" s="2" t="s">
@@ -1113,7 +1112,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A6" s="12">
         <v>4</v>
       </c>
@@ -1202,7 +1201,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A7" s="12">
         <v>5</v>
       </c>
@@ -1254,7 +1253,7 @@
       <c r="Q7" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="R7" s="21" t="s">
+      <c r="R7" s="7" t="s">
         <v>6</v>
       </c>
       <c r="S7" s="2" t="s">
@@ -1288,7 +1287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A8" s="12">
         <v>6</v>
       </c>
@@ -1337,7 +1336,7 @@
       <c r="P8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="Q8" s="20" t="s">
+      <c r="Q8" s="7" t="s">
         <v>6</v>
       </c>
       <c r="R8" s="7" t="s">
@@ -1377,7 +1376,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A9" s="12">
         <v>7</v>
       </c>
@@ -1466,7 +1465,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A10" s="12">
         <v>8</v>
       </c>
@@ -1491,7 +1490,7 @@
       <c r="H10" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="I10" s="7" t="s">
+      <c r="I10" s="21" t="s">
         <v>6</v>
       </c>
       <c r="J10" s="7" t="s">
@@ -1518,7 +1517,7 @@
       <c r="Q10" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="R10" s="7" t="s">
+      <c r="R10" s="21" t="s">
         <v>6</v>
       </c>
       <c r="S10" s="7" t="s">
@@ -1552,7 +1551,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A11" s="12">
         <v>9</v>
       </c>
@@ -1638,7 +1637,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A12" s="12">
         <v>10</v>
       </c>
@@ -1724,7 +1723,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A13" s="12">
         <v>11</v>
       </c>
@@ -1734,7 +1733,7 @@
       <c r="C13" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="21" t="s">
         <v>12</v>
       </c>
       <c r="E13" s="2" t="s">
@@ -1788,7 +1787,7 @@
       <c r="U13" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="V13" s="7" t="s">
+      <c r="V13" s="20" t="s">
         <v>6</v>
       </c>
       <c r="W13" s="7" t="s">
@@ -1810,11 +1809,11 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A14" s="12">
         <v>12</v>
       </c>
-      <c r="B14" s="21" t="s">
+      <c r="B14" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C14" s="7" t="s">
@@ -1829,7 +1828,7 @@
       <c r="F14" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G14" s="21" t="s">
+      <c r="G14" s="7" t="s">
         <v>6</v>
       </c>
       <c r="H14" s="7" t="s">
@@ -1896,7 +1895,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A15" s="12">
         <v>13</v>
       </c>
@@ -1960,13 +1959,13 @@
       <c r="U15" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="V15" s="7" t="s">
+      <c r="V15" s="20" t="s">
         <v>6</v>
       </c>
       <c r="W15" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="X15" s="23" t="s">
+      <c r="X15" s="22" t="s">
         <v>6</v>
       </c>
       <c r="Y15" s="7" t="s">
@@ -1982,7 +1981,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A16" s="12">
         <v>14</v>
       </c>
@@ -2068,7 +2067,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A17" s="12">
         <v>15</v>
       </c>
@@ -2154,7 +2153,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A18" s="12">
         <v>16</v>
       </c>
@@ -2240,7 +2239,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A19" s="12">
         <v>17</v>
       </c>
@@ -2326,7 +2325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A20" s="12">
         <v>18</v>
       </c>
@@ -2412,7 +2411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A21" s="12">
         <v>19</v>
       </c>
@@ -2498,7 +2497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A22" s="12">
         <v>20</v>
       </c>
@@ -2584,7 +2583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A23" s="12">
         <v>21</v>
       </c>
@@ -2670,7 +2669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A24" s="12">
         <v>22</v>
       </c>
@@ -2756,7 +2755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A25" s="12">
         <v>23</v>
       </c>
@@ -2842,7 +2841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A26" s="12">
         <v>24</v>
       </c>
@@ -2928,7 +2927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A27" s="12">
         <v>25</v>
       </c>
@@ -2977,7 +2976,7 @@
       <c r="P27" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="Q27" s="7" t="s">
+      <c r="Q27" s="21" t="s">
         <v>6</v>
       </c>
       <c r="R27" s="7" t="s">

</xml_diff>